<commit_message>
//Changed to pickup store
</commit_message>
<xml_diff>
--- a/Automation_TestCases.xlsx
+++ b/Automation_TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t xml:space="preserve">Exp Total Price</t>
   </si>
@@ -108,6 +108,45 @@
   </si>
   <si>
     <t xml:space="preserve">Verify cart amount with review page payable amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandatory fields validation on review page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Everyday Value Offer text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verify alert in deal of 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> step </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify alert if select no pizza</t>
   </si>
 </sst>
 </file>
@@ -117,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -141,6 +180,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -227,9 +273,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,17 +310,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,6 +520,38 @@
         <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>